<commit_message>
added parameter change output
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA987A0C-3D30-4C50-AE5D-B2C6317135C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4224C2F-1F6B-45E5-8DC2-84C4DF01948F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{82D83D76-C0B7-4FC5-9E46-F06C8E4A2643}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="374">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -449,9 +449,6 @@
     <t>2trial</t>
   </si>
   <si>
-    <t>2+</t>
-  </si>
-  <si>
     <t>rear-end</t>
   </si>
   <si>
@@ -1152,6 +1149,15 @@
   </si>
   <si>
     <t>clip leading to topple</t>
+  </si>
+  <si>
+    <t>intersection</t>
+  </si>
+  <si>
+    <t>3+</t>
+  </si>
+  <si>
+    <t>rear-end, t-bone</t>
   </si>
 </sst>
 </file>
@@ -1570,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD03C49-7425-41FE-9DB8-DAD708A39D50}">
   <dimension ref="A1:L203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E78" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,7 +1596,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1733,13 +1739,13 @@
         <v>136</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>137</v>
+        <v>372</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>373</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -1752,6 +1758,9 @@
       </c>
       <c r="K5" t="s">
         <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1794,13 +1803,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D7" t="s">
         <v>79</v>
@@ -1815,7 +1824,7 @@
         <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K7" t="s">
         <v>11</v>
@@ -1861,7 +1870,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="3"/>
       <c r="H9" t="s">
@@ -1914,7 +1923,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="3"/>
     </row>
@@ -1958,7 +1967,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13" s="3"/>
       <c r="J13" t="s">
@@ -2008,7 +2017,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" s="3"/>
       <c r="K15" t="s">
@@ -2055,11 +2064,11 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K17" t="s">
         <v>13</v>
@@ -2105,7 +2114,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="3">
         <v>2</v>
@@ -2163,7 +2172,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21" s="3"/>
       <c r="K21" t="s">
@@ -2210,7 +2219,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" s="3"/>
     </row>
@@ -2254,13 +2263,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -2275,7 +2284,7 @@
         <v>79</v>
       </c>
       <c r="H25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
@@ -2321,37 +2330,37 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" s="3">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E27" t="s">
+        <v>358</v>
+      </c>
+      <c r="F27" t="s">
+        <v>358</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" t="s">
+        <v>358</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" t="s">
         <v>359</v>
-      </c>
-      <c r="E27" t="s">
-        <v>359</v>
-      </c>
-      <c r="F27" t="s">
-        <v>359</v>
-      </c>
-      <c r="G27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" t="s">
-        <v>359</v>
-      </c>
-      <c r="I27" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2394,13 +2403,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2415,7 +2424,7 @@
         <v>13</v>
       </c>
       <c r="H29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
@@ -2424,7 +2433,7 @@
         <v>13</v>
       </c>
       <c r="L29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2467,11 +2476,11 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B31" s="3"/>
       <c r="L31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2514,34 +2523,34 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C33" t="s">
+        <v>278</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>360</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" t="s">
         <v>279</v>
-      </c>
-      <c r="C33" t="s">
-        <v>279</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" t="s">
-        <v>361</v>
-      </c>
-      <c r="I33" t="s">
-        <v>11</v>
-      </c>
-      <c r="L33" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2584,11 +2593,11 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B35" s="3"/>
       <c r="L35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2631,13 +2640,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -2658,7 +2667,7 @@
         <v>25</v>
       </c>
       <c r="L37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2701,37 +2710,37 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>278</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>361</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" t="s">
+        <v>13</v>
+      </c>
+      <c r="L39" t="s">
         <v>279</v>
-      </c>
-      <c r="D39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" t="s">
-        <v>362</v>
-      </c>
-      <c r="I39" t="s">
-        <v>11</v>
-      </c>
-      <c r="K39" t="s">
-        <v>13</v>
-      </c>
-      <c r="L39" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2774,13 +2783,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -2795,7 +2804,7 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I41" t="s">
         <v>11</v>
@@ -2807,7 +2816,7 @@
         <v>11</v>
       </c>
       <c r="L41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2847,37 +2856,37 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C43" t="s">
+        <v>278</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" t="s">
+        <v>278</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" t="s">
+        <v>13</v>
+      </c>
+      <c r="L43" t="s">
         <v>279</v>
-      </c>
-      <c r="C43" t="s">
-        <v>279</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" t="s">
-        <v>279</v>
-      </c>
-      <c r="I43" t="s">
-        <v>11</v>
-      </c>
-      <c r="K43" t="s">
-        <v>13</v>
-      </c>
-      <c r="L43" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2920,37 +2929,37 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C45" t="s">
+        <v>278</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>278</v>
+      </c>
+      <c r="I45" t="s">
+        <v>11</v>
+      </c>
+      <c r="K45" t="s">
+        <v>11</v>
+      </c>
+      <c r="L45" t="s">
         <v>279</v>
-      </c>
-      <c r="C45" t="s">
-        <v>279</v>
-      </c>
-      <c r="D45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" t="s">
-        <v>279</v>
-      </c>
-      <c r="I45" t="s">
-        <v>11</v>
-      </c>
-      <c r="K45" t="s">
-        <v>11</v>
-      </c>
-      <c r="L45" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2993,7 +3002,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
@@ -3057,7 +3066,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B49" s="3"/>
     </row>
@@ -3101,7 +3110,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B51" s="3"/>
     </row>
@@ -3145,13 +3154,13 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B53" s="3">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D53" t="s">
         <v>13</v>
@@ -3166,13 +3175,13 @@
         <v>13</v>
       </c>
       <c r="H53" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I53" t="s">
         <v>11</v>
       </c>
       <c r="L53" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3215,16 +3224,16 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D55" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -3279,7 +3288,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B57" s="3"/>
     </row>
@@ -3323,7 +3332,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B59" s="3"/>
     </row>
@@ -3367,7 +3376,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B61" s="3"/>
     </row>
@@ -3411,13 +3420,13 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B63" s="3">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D63" t="s">
         <v>79</v>
@@ -3475,7 +3484,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -3527,7 +3536,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B67" s="3"/>
     </row>
@@ -3571,31 +3580,31 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C69" t="s">
+        <v>278</v>
+      </c>
+      <c r="D69" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" t="s">
+        <v>11</v>
+      </c>
+      <c r="I69" t="s">
+        <v>11</v>
+      </c>
+      <c r="L69" t="s">
         <v>279</v>
-      </c>
-      <c r="C69" t="s">
-        <v>279</v>
-      </c>
-      <c r="D69" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s">
-        <v>11</v>
-      </c>
-      <c r="G69" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" t="s">
-        <v>11</v>
-      </c>
-      <c r="L69" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3638,13 +3647,13 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B71" s="3">
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D71" t="s">
         <v>79</v>
@@ -3702,7 +3711,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B73" s="3">
         <v>2</v>
@@ -3763,7 +3772,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B75" s="3">
         <v>1</v>
@@ -3784,7 +3793,7 @@
         <v>13</v>
       </c>
       <c r="H75" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I75" t="s">
         <v>11</v>
@@ -3836,13 +3845,13 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C77" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D77" t="s">
         <v>11</v>
@@ -3857,7 +3866,7 @@
         <v>11</v>
       </c>
       <c r="H77" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I77" t="s">
         <v>11</v>
@@ -3869,7 +3878,7 @@
         <v>11</v>
       </c>
       <c r="L77" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3912,13 +3921,13 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B79" s="3">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D79" t="s">
         <v>79</v>
@@ -3927,7 +3936,7 @@
         <v>79</v>
       </c>
       <c r="F79" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G79" t="s">
         <v>13</v>
@@ -3973,7 +3982,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B81" s="3"/>
     </row>
@@ -4017,7 +4026,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B83" s="3"/>
     </row>
@@ -4061,28 +4070,28 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B85" s="3">
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D85" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E85" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F85" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G85" t="s">
         <v>13</v>
       </c>
       <c r="H85" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I85" t="s">
         <v>11</v>
@@ -4131,7 +4140,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B87" s="3"/>
     </row>
@@ -4175,7 +4184,7 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B89" s="3">
         <v>2</v>
@@ -4196,7 +4205,7 @@
         <v>13</v>
       </c>
       <c r="H89" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I89" t="s">
         <v>11</v>
@@ -4242,7 +4251,7 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B91" s="3"/>
     </row>
@@ -4286,7 +4295,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B93" s="3"/>
     </row>
@@ -4330,13 +4339,13 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B95" s="3">
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D95" t="s">
         <v>79</v>
@@ -4400,7 +4409,7 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B97" s="3"/>
     </row>
@@ -4444,13 +4453,13 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C99" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
@@ -4465,13 +4474,13 @@
         <v>11</v>
       </c>
       <c r="H99" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I99" t="s">
         <v>11</v>
       </c>
       <c r="L99" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -4482,45 +4491,45 @@
         <v>2</v>
       </c>
       <c r="C100" t="s">
+        <v>190</v>
+      </c>
+      <c r="D100" t="s">
+        <v>11</v>
+      </c>
+      <c r="E100" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100" t="s">
+        <v>13</v>
+      </c>
+      <c r="H100" t="s">
         <v>191</v>
       </c>
-      <c r="D100" t="s">
-        <v>11</v>
-      </c>
-      <c r="E100" t="s">
-        <v>11</v>
-      </c>
-      <c r="F100" t="s">
-        <v>11</v>
-      </c>
-      <c r="G100" t="s">
-        <v>13</v>
-      </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J100" t="s">
         <v>192</v>
       </c>
-      <c r="I100" t="s">
-        <v>11</v>
-      </c>
-      <c r="J100" t="s">
+      <c r="K100" t="s">
+        <v>11</v>
+      </c>
+      <c r="L100" t="s">
         <v>193</v>
-      </c>
-      <c r="K100" t="s">
-        <v>11</v>
-      </c>
-      <c r="L100" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B101" s="3">
         <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D101" t="s">
         <v>13</v>
@@ -4546,22 +4555,22 @@
         <v>2</v>
       </c>
       <c r="C102" t="s">
+        <v>194</v>
+      </c>
+      <c r="D102" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" t="s">
+        <v>11</v>
+      </c>
+      <c r="G102" t="s">
+        <v>11</v>
+      </c>
+      <c r="H102" t="s">
         <v>195</v>
-      </c>
-      <c r="D102" t="s">
-        <v>11</v>
-      </c>
-      <c r="E102" t="s">
-        <v>11</v>
-      </c>
-      <c r="F102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G102" t="s">
-        <v>11</v>
-      </c>
-      <c r="H102" t="s">
-        <v>196</v>
       </c>
       <c r="I102" t="s">
         <v>11</v>
@@ -4573,18 +4582,18 @@
         <v>11</v>
       </c>
       <c r="L102" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B103" s="3">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D103" t="s">
         <v>13</v>
@@ -4599,7 +4608,7 @@
         <v>13</v>
       </c>
       <c r="H103" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I103" t="s">
         <v>11</v>
@@ -4643,12 +4652,12 @@
         <v>11</v>
       </c>
       <c r="L104" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B105" s="3">
         <v>2</v>
@@ -4669,7 +4678,7 @@
         <v>13</v>
       </c>
       <c r="H105" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -4680,22 +4689,22 @@
         <v>2</v>
       </c>
       <c r="C106" t="s">
+        <v>198</v>
+      </c>
+      <c r="D106" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" t="s">
+        <v>11</v>
+      </c>
+      <c r="G106" t="s">
+        <v>13</v>
+      </c>
+      <c r="H106" t="s">
         <v>199</v>
-      </c>
-      <c r="D106" t="s">
-        <v>11</v>
-      </c>
-      <c r="E106" t="s">
-        <v>11</v>
-      </c>
-      <c r="F106" t="s">
-        <v>11</v>
-      </c>
-      <c r="G106" t="s">
-        <v>13</v>
-      </c>
-      <c r="H106" t="s">
-        <v>200</v>
       </c>
       <c r="I106" t="s">
         <v>11</v>
@@ -4707,22 +4716,22 @@
         <v>11</v>
       </c>
       <c r="L106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B107" s="3"/>
       <c r="H107" t="s">
+        <v>349</v>
+      </c>
+      <c r="J107" t="s">
         <v>350</v>
       </c>
-      <c r="J107" t="s">
+      <c r="L107" t="s">
         <v>351</v>
-      </c>
-      <c r="L107" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
@@ -4733,7 +4742,7 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D108" t="s">
         <v>13</v>
@@ -4748,7 +4757,7 @@
         <v>13</v>
       </c>
       <c r="H108" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I108" t="s">
         <v>13</v>
@@ -4760,22 +4769,22 @@
         <v>11</v>
       </c>
       <c r="L108" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B109" s="3"/>
       <c r="H109" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J109" t="s">
+        <v>350</v>
+      </c>
+      <c r="L109" t="s">
         <v>351</v>
-      </c>
-      <c r="L109" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -4813,12 +4822,12 @@
         <v>11</v>
       </c>
       <c r="L110" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B111" s="3"/>
     </row>
@@ -4845,7 +4854,7 @@
         <v>13</v>
       </c>
       <c r="H112" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I112" t="s">
         <v>11</v>
@@ -4857,12 +4866,12 @@
         <v>11</v>
       </c>
       <c r="L112" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B113" s="3"/>
     </row>
@@ -4874,22 +4883,22 @@
         <v>2</v>
       </c>
       <c r="C114" t="s">
+        <v>205</v>
+      </c>
+      <c r="D114" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" t="s">
+        <v>11</v>
+      </c>
+      <c r="G114" t="s">
+        <v>11</v>
+      </c>
+      <c r="H114" t="s">
         <v>206</v>
-      </c>
-      <c r="D114" t="s">
-        <v>11</v>
-      </c>
-      <c r="E114" t="s">
-        <v>11</v>
-      </c>
-      <c r="F114" t="s">
-        <v>11</v>
-      </c>
-      <c r="G114" t="s">
-        <v>11</v>
-      </c>
-      <c r="H114" t="s">
-        <v>207</v>
       </c>
       <c r="I114" t="s">
         <v>11</v>
@@ -4901,12 +4910,12 @@
         <v>11</v>
       </c>
       <c r="L114" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B115" s="3"/>
     </row>
@@ -4918,7 +4927,7 @@
         <v>2</v>
       </c>
       <c r="C116" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D116" t="s">
         <v>13</v>
@@ -4933,7 +4942,7 @@
         <v>13</v>
       </c>
       <c r="H116" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I116" t="s">
         <v>11</v>
@@ -4945,12 +4954,12 @@
         <v>11</v>
       </c>
       <c r="L116" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B117" s="3"/>
     </row>
@@ -4989,12 +4998,12 @@
         <v>11</v>
       </c>
       <c r="L118" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B119" s="3"/>
     </row>
@@ -5033,12 +5042,12 @@
         <v>11</v>
       </c>
       <c r="L120" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B121" s="3"/>
     </row>
@@ -5071,18 +5080,18 @@
         <v>11</v>
       </c>
       <c r="J122" t="s">
+        <v>211</v>
+      </c>
+      <c r="K122" t="s">
+        <v>11</v>
+      </c>
+      <c r="L122" t="s">
         <v>212</v>
-      </c>
-      <c r="K122" t="s">
-        <v>11</v>
-      </c>
-      <c r="L122" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B123" s="3"/>
     </row>
@@ -5094,7 +5103,7 @@
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D124" t="s">
         <v>13</v>
@@ -5121,12 +5130,12 @@
         <v>11</v>
       </c>
       <c r="L124" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B125" s="3"/>
     </row>
@@ -5153,7 +5162,7 @@
         <v>13</v>
       </c>
       <c r="H126" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I126" t="s">
         <v>11</v>
@@ -5165,12 +5174,12 @@
         <v>11</v>
       </c>
       <c r="L126" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B127" s="3"/>
     </row>
@@ -5182,7 +5191,7 @@
         <v>2</v>
       </c>
       <c r="C128" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D128" t="s">
         <v>13</v>
@@ -5197,7 +5206,7 @@
         <v>13</v>
       </c>
       <c r="H128" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I128" t="s">
         <v>11</v>
@@ -5209,12 +5218,12 @@
         <v>11</v>
       </c>
       <c r="L128" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B129" s="3"/>
     </row>
@@ -5226,39 +5235,39 @@
         <v>2</v>
       </c>
       <c r="C130" t="s">
+        <v>219</v>
+      </c>
+      <c r="D130" t="s">
+        <v>13</v>
+      </c>
+      <c r="E130" t="s">
+        <v>13</v>
+      </c>
+      <c r="F130" t="s">
+        <v>11</v>
+      </c>
+      <c r="G130" t="s">
+        <v>13</v>
+      </c>
+      <c r="H130" t="s">
         <v>220</v>
       </c>
-      <c r="D130" t="s">
-        <v>13</v>
-      </c>
-      <c r="E130" t="s">
-        <v>13</v>
-      </c>
-      <c r="F130" t="s">
-        <v>11</v>
-      </c>
-      <c r="G130" t="s">
-        <v>13</v>
-      </c>
-      <c r="H130" t="s">
+      <c r="I130" t="s">
+        <v>11</v>
+      </c>
+      <c r="J130" t="s">
         <v>221</v>
       </c>
-      <c r="I130" t="s">
-        <v>11</v>
-      </c>
-      <c r="J130" t="s">
+      <c r="K130" t="s">
+        <v>11</v>
+      </c>
+      <c r="L130" t="s">
         <v>222</v>
-      </c>
-      <c r="K130" t="s">
-        <v>11</v>
-      </c>
-      <c r="L130" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B131" s="3"/>
     </row>
@@ -5285,24 +5294,24 @@
         <v>13</v>
       </c>
       <c r="H132" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I132" t="s">
         <v>11</v>
       </c>
       <c r="J132" t="s">
+        <v>223</v>
+      </c>
+      <c r="K132" t="s">
+        <v>11</v>
+      </c>
+      <c r="L132" t="s">
         <v>224</v>
-      </c>
-      <c r="K132" t="s">
-        <v>11</v>
-      </c>
-      <c r="L132" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B133" s="3"/>
     </row>
@@ -5314,22 +5323,22 @@
         <v>1</v>
       </c>
       <c r="C134" t="s">
+        <v>225</v>
+      </c>
+      <c r="D134" t="s">
+        <v>13</v>
+      </c>
+      <c r="E134" t="s">
+        <v>13</v>
+      </c>
+      <c r="F134" t="s">
+        <v>11</v>
+      </c>
+      <c r="G134" t="s">
+        <v>13</v>
+      </c>
+      <c r="H134" t="s">
         <v>226</v>
-      </c>
-      <c r="D134" t="s">
-        <v>13</v>
-      </c>
-      <c r="E134" t="s">
-        <v>13</v>
-      </c>
-      <c r="F134" t="s">
-        <v>11</v>
-      </c>
-      <c r="G134" t="s">
-        <v>13</v>
-      </c>
-      <c r="H134" t="s">
-        <v>227</v>
       </c>
       <c r="I134" t="s">
         <v>11</v>
@@ -5341,19 +5350,19 @@
         <v>11</v>
       </c>
       <c r="L134" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B135" s="3"/>
       <c r="J135" t="s">
         <v>25</v>
       </c>
       <c r="L135" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -5364,7 +5373,7 @@
         <v>4</v>
       </c>
       <c r="C136" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D136" t="s">
         <v>13</v>
@@ -5379,24 +5388,24 @@
         <v>13</v>
       </c>
       <c r="H136" t="s">
+        <v>228</v>
+      </c>
+      <c r="I136" t="s">
+        <v>11</v>
+      </c>
+      <c r="J136" t="s">
         <v>229</v>
       </c>
-      <c r="I136" t="s">
-        <v>11</v>
-      </c>
-      <c r="J136" t="s">
+      <c r="K136" t="s">
+        <v>11</v>
+      </c>
+      <c r="L136" t="s">
         <v>230</v>
-      </c>
-      <c r="K136" t="s">
-        <v>11</v>
-      </c>
-      <c r="L136" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B137" s="3"/>
     </row>
@@ -5423,7 +5432,7 @@
         <v>13</v>
       </c>
       <c r="H138" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I138" t="s">
         <v>11</v>
@@ -5435,12 +5444,12 @@
         <v>11</v>
       </c>
       <c r="L138" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B139" s="3"/>
     </row>
@@ -5449,10 +5458,10 @@
         <v>70</v>
       </c>
       <c r="B140" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C140" t="s">
         <v>234</v>
-      </c>
-      <c r="C140" t="s">
-        <v>235</v>
       </c>
       <c r="D140" t="s">
         <v>11</v>
@@ -5479,16 +5488,16 @@
         <v>11</v>
       </c>
       <c r="L140" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B141" s="3"/>
       <c r="L141" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
@@ -5499,22 +5508,22 @@
         <v>2</v>
       </c>
       <c r="C142" t="s">
+        <v>236</v>
+      </c>
+      <c r="D142" t="s">
+        <v>13</v>
+      </c>
+      <c r="E142" t="s">
+        <v>13</v>
+      </c>
+      <c r="F142" t="s">
+        <v>11</v>
+      </c>
+      <c r="G142" t="s">
+        <v>13</v>
+      </c>
+      <c r="H142" t="s">
         <v>237</v>
-      </c>
-      <c r="D142" t="s">
-        <v>13</v>
-      </c>
-      <c r="E142" t="s">
-        <v>13</v>
-      </c>
-      <c r="F142" t="s">
-        <v>11</v>
-      </c>
-      <c r="G142" t="s">
-        <v>13</v>
-      </c>
-      <c r="H142" t="s">
-        <v>238</v>
       </c>
       <c r="I142" t="s">
         <v>11</v>
@@ -5526,12 +5535,12 @@
         <v>11</v>
       </c>
       <c r="L142" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B143" s="3"/>
     </row>
@@ -5558,7 +5567,7 @@
         <v>13</v>
       </c>
       <c r="H144" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I144" t="s">
         <v>11</v>
@@ -5570,12 +5579,12 @@
         <v>11</v>
       </c>
       <c r="L144" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B145" s="3"/>
     </row>
@@ -5587,7 +5596,7 @@
         <v>2</v>
       </c>
       <c r="C146" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D146" t="s">
         <v>79</v>
@@ -5602,7 +5611,7 @@
         <v>13</v>
       </c>
       <c r="H146" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I146" t="s">
         <v>11</v>
@@ -5614,12 +5623,12 @@
         <v>11</v>
       </c>
       <c r="L146" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B147" s="3"/>
     </row>
@@ -5631,22 +5640,22 @@
         <v>2</v>
       </c>
       <c r="C148" t="s">
+        <v>243</v>
+      </c>
+      <c r="D148" t="s">
+        <v>13</v>
+      </c>
+      <c r="E148" t="s">
+        <v>13</v>
+      </c>
+      <c r="F148" t="s">
+        <v>11</v>
+      </c>
+      <c r="G148" t="s">
+        <v>13</v>
+      </c>
+      <c r="H148" t="s">
         <v>244</v>
-      </c>
-      <c r="D148" t="s">
-        <v>13</v>
-      </c>
-      <c r="E148" t="s">
-        <v>13</v>
-      </c>
-      <c r="F148" t="s">
-        <v>11</v>
-      </c>
-      <c r="G148" t="s">
-        <v>13</v>
-      </c>
-      <c r="H148" t="s">
-        <v>245</v>
       </c>
       <c r="I148" t="s">
         <v>11</v>
@@ -5658,12 +5667,12 @@
         <v>11</v>
       </c>
       <c r="L148" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B149" s="3"/>
     </row>
@@ -5690,7 +5699,7 @@
         <v>11</v>
       </c>
       <c r="H150" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I150" t="s">
         <v>11</v>
@@ -5702,12 +5711,12 @@
         <v>13</v>
       </c>
       <c r="L150" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B151" s="3"/>
     </row>
@@ -5746,12 +5755,12 @@
         <v>11</v>
       </c>
       <c r="L152" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B153" s="3"/>
     </row>
@@ -5790,12 +5799,12 @@
         <v>11</v>
       </c>
       <c r="L154" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B155" s="3"/>
     </row>
@@ -5822,7 +5831,7 @@
         <v>13</v>
       </c>
       <c r="H156" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I156" t="s">
         <v>11</v>
@@ -5834,12 +5843,12 @@
         <v>11</v>
       </c>
       <c r="L156" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B157" s="3"/>
     </row>
@@ -5866,7 +5875,7 @@
         <v>13</v>
       </c>
       <c r="H158" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I158" t="s">
         <v>11</v>
@@ -5878,12 +5887,12 @@
         <v>11</v>
       </c>
       <c r="L158" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B159" s="3"/>
     </row>
@@ -5910,7 +5919,7 @@
         <v>11</v>
       </c>
       <c r="H160" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I160" t="s">
         <v>11</v>
@@ -5922,12 +5931,12 @@
         <v>11</v>
       </c>
       <c r="L160" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B161" s="3"/>
     </row>
@@ -5954,24 +5963,24 @@
         <v>11</v>
       </c>
       <c r="H162" t="s">
+        <v>254</v>
+      </c>
+      <c r="I162" t="s">
+        <v>11</v>
+      </c>
+      <c r="J162" t="s">
+        <v>229</v>
+      </c>
+      <c r="K162" t="s">
+        <v>11</v>
+      </c>
+      <c r="L162" t="s">
         <v>255</v>
-      </c>
-      <c r="I162" t="s">
-        <v>11</v>
-      </c>
-      <c r="J162" t="s">
-        <v>230</v>
-      </c>
-      <c r="K162" t="s">
-        <v>11</v>
-      </c>
-      <c r="L162" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B163" s="3"/>
     </row>
@@ -5998,7 +6007,7 @@
         <v>11</v>
       </c>
       <c r="H164" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I164" t="s">
         <v>11</v>
@@ -6010,12 +6019,12 @@
         <v>11</v>
       </c>
       <c r="L164" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B165" s="3"/>
     </row>
@@ -6027,7 +6036,7 @@
         <v>2</v>
       </c>
       <c r="C166" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D166" t="s">
         <v>79</v>
@@ -6054,12 +6063,12 @@
         <v>11</v>
       </c>
       <c r="L166" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B167" s="3"/>
     </row>
@@ -6071,7 +6080,7 @@
         <v>2</v>
       </c>
       <c r="C168" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D168" t="s">
         <v>11</v>
@@ -6086,7 +6095,7 @@
         <v>13</v>
       </c>
       <c r="H168" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I168" t="s">
         <v>11</v>
@@ -6098,12 +6107,12 @@
         <v>11</v>
       </c>
       <c r="L168" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B169" s="3"/>
     </row>
@@ -6130,7 +6139,7 @@
         <v>11</v>
       </c>
       <c r="H170" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I170" t="s">
         <v>11</v>
@@ -6142,12 +6151,12 @@
         <v>13</v>
       </c>
       <c r="L170" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B171" s="3"/>
     </row>
@@ -6174,7 +6183,7 @@
         <v>13</v>
       </c>
       <c r="H172" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I172" t="s">
         <v>11</v>
@@ -6186,12 +6195,12 @@
         <v>11</v>
       </c>
       <c r="L172" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B173" s="3"/>
     </row>
@@ -6203,7 +6212,7 @@
         <v>2</v>
       </c>
       <c r="C174" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D174" t="s">
         <v>11</v>
@@ -6218,7 +6227,7 @@
         <v>13</v>
       </c>
       <c r="H174" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I174" t="s">
         <v>11</v>
@@ -6230,12 +6239,12 @@
         <v>11</v>
       </c>
       <c r="L174" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B175" s="3"/>
     </row>
@@ -6262,7 +6271,7 @@
         <v>13</v>
       </c>
       <c r="H176" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I176" t="s">
         <v>11</v>
@@ -6274,12 +6283,12 @@
         <v>11</v>
       </c>
       <c r="L176" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B177" s="3"/>
     </row>
@@ -6306,7 +6315,7 @@
         <v>11</v>
       </c>
       <c r="H178" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I178" t="s">
         <v>11</v>
@@ -6318,12 +6327,12 @@
         <v>11</v>
       </c>
       <c r="L178" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B179" s="3"/>
     </row>
@@ -6350,7 +6359,7 @@
         <v>13</v>
       </c>
       <c r="H180" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I180" t="s">
         <v>11</v>
@@ -6362,12 +6371,12 @@
         <v>11</v>
       </c>
       <c r="L180" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B181" s="3"/>
     </row>
@@ -6394,7 +6403,7 @@
         <v>13</v>
       </c>
       <c r="H182" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I182" t="s">
         <v>11</v>
@@ -6406,12 +6415,12 @@
         <v>11</v>
       </c>
       <c r="L182" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B183" s="3"/>
     </row>
@@ -6438,7 +6447,7 @@
         <v>13</v>
       </c>
       <c r="H184" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I184" t="s">
         <v>11</v>
@@ -6450,12 +6459,12 @@
         <v>11</v>
       </c>
       <c r="L184" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B185" s="3"/>
     </row>
@@ -6467,7 +6476,7 @@
         <v>1</v>
       </c>
       <c r="C186" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D186" t="s">
         <v>11</v>
@@ -6482,7 +6491,7 @@
         <v>11</v>
       </c>
       <c r="H186" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I186" t="s">
         <v>11</v>
@@ -6494,12 +6503,12 @@
         <v>11</v>
       </c>
       <c r="L186" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B187" s="3"/>
     </row>
@@ -6511,7 +6520,7 @@
         <v>0</v>
       </c>
       <c r="C188" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D188" t="s">
         <v>11</v>
@@ -6526,7 +6535,7 @@
         <v>11</v>
       </c>
       <c r="H188" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I188" t="s">
         <v>11</v>
@@ -6538,12 +6547,12 @@
         <v>11</v>
       </c>
       <c r="L188" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B189" s="3"/>
     </row>
@@ -6552,7 +6561,7 @@
         <v>95</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C190" t="s">
         <v>104</v>
@@ -6582,12 +6591,12 @@
         <v>11</v>
       </c>
       <c r="L190" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B191" s="3"/>
     </row>
@@ -6596,7 +6605,7 @@
         <v>96</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C192" t="s">
         <v>104</v>
@@ -6626,12 +6635,12 @@
         <v>11</v>
       </c>
       <c r="L192" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B193" s="3"/>
     </row>
@@ -6658,24 +6667,24 @@
         <v>13</v>
       </c>
       <c r="H194" t="s">
+        <v>283</v>
+      </c>
+      <c r="I194" t="s">
+        <v>11</v>
+      </c>
+      <c r="J194" t="s">
         <v>284</v>
       </c>
-      <c r="I194" t="s">
-        <v>11</v>
-      </c>
-      <c r="J194" t="s">
+      <c r="K194" t="s">
+        <v>11</v>
+      </c>
+      <c r="L194" t="s">
         <v>285</v>
-      </c>
-      <c r="K194" t="s">
-        <v>11</v>
-      </c>
-      <c r="L194" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B195" s="3"/>
     </row>
@@ -6702,24 +6711,24 @@
         <v>13</v>
       </c>
       <c r="H196" t="s">
+        <v>286</v>
+      </c>
+      <c r="I196" t="s">
+        <v>11</v>
+      </c>
+      <c r="J196" t="s">
         <v>287</v>
       </c>
-      <c r="I196" t="s">
-        <v>11</v>
-      </c>
-      <c r="J196" t="s">
+      <c r="K196" t="s">
+        <v>11</v>
+      </c>
+      <c r="L196" t="s">
         <v>288</v>
-      </c>
-      <c r="K196" t="s">
-        <v>11</v>
-      </c>
-      <c r="L196" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B197" s="3"/>
     </row>
@@ -6731,7 +6740,7 @@
         <v>2</v>
       </c>
       <c r="C198" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D198" t="s">
         <v>11</v>
@@ -6746,7 +6755,7 @@
         <v>13</v>
       </c>
       <c r="H198" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I198" t="s">
         <v>11</v>
@@ -6758,12 +6767,12 @@
         <v>11</v>
       </c>
       <c r="L198" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B199" s="3"/>
     </row>
@@ -6775,7 +6784,7 @@
         <v>2</v>
       </c>
       <c r="C200" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D200" t="s">
         <v>11</v>
@@ -6790,24 +6799,24 @@
         <v>13</v>
       </c>
       <c r="H200" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I200" t="s">
         <v>11</v>
       </c>
       <c r="J200" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K200" t="s">
         <v>11</v>
       </c>
       <c r="L200" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B201" s="3"/>
     </row>
@@ -6834,24 +6843,24 @@
         <v>13</v>
       </c>
       <c r="H202" t="s">
+        <v>292</v>
+      </c>
+      <c r="I202" t="s">
+        <v>11</v>
+      </c>
+      <c r="J202" t="s">
+        <v>211</v>
+      </c>
+      <c r="K202" t="s">
+        <v>11</v>
+      </c>
+      <c r="L202" t="s">
         <v>293</v>
-      </c>
-      <c r="I202" t="s">
-        <v>11</v>
-      </c>
-      <c r="J202" t="s">
-        <v>212</v>
-      </c>
-      <c r="K202" t="s">
-        <v>11</v>
-      </c>
-      <c r="L202" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B203" s="3"/>
     </row>

</xml_diff>

<commit_message>
added trials thru 80
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4224C2F-1F6B-45E5-8DC2-84C4DF01948F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB056D17-F9FC-45E9-8193-4EDBA2509454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{82D83D76-C0B7-4FC5-9E46-F06C8E4A2643}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82D83D76-C0B7-4FC5-9E46-F06C8E4A2643}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="382">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -1097,9 +1097,6 @@
     <t>White suv, fire truck</t>
   </si>
   <si>
-    <t>Urban, pedrestrian crossing</t>
-  </si>
-  <si>
     <t>Parking lot</t>
   </si>
   <si>
@@ -1158,6 +1155,33 @@
   </si>
   <si>
     <t>rear-end, t-bone</t>
+  </si>
+  <si>
+    <t>one-vehicle collision</t>
+  </si>
+  <si>
+    <t>Motorcycle or scooter?</t>
+  </si>
+  <si>
+    <t>sudden overturn</t>
+  </si>
+  <si>
+    <t>Urban, pedrestrian crossing, no accident occurred</t>
+  </si>
+  <si>
+    <t>t-bone (train)</t>
+  </si>
+  <si>
+    <t>truck, train</t>
+  </si>
+  <si>
+    <t>AI gets this one spot-on</t>
+  </si>
+  <si>
+    <t>Loss of control</t>
+  </si>
+  <si>
+    <t>2 or 3</t>
   </si>
 </sst>
 </file>
@@ -1576,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD03C49-7425-41FE-9DB8-DAD708A39D50}">
   <dimension ref="A1:L203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,10 +1763,10 @@
         <v>136</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C5" t="s">
         <v>372</v>
-      </c>
-      <c r="C5" t="s">
-        <v>373</v>
       </c>
       <c r="D5" t="s">
         <v>79</v>
@@ -1760,7 +1784,7 @@
         <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1809,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D7" t="s">
         <v>79</v>
@@ -1824,7 +1848,7 @@
         <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K7" t="s">
         <v>11</v>
@@ -2269,7 +2293,7 @@
         <v>278</v>
       </c>
       <c r="C25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -2339,28 +2363,28 @@
         <v>278</v>
       </c>
       <c r="D27" t="s">
+        <v>357</v>
+      </c>
+      <c r="E27" t="s">
+        <v>357</v>
+      </c>
+      <c r="F27" t="s">
+        <v>357</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" t="s">
+        <v>357</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" t="s">
         <v>358</v>
-      </c>
-      <c r="E27" t="s">
-        <v>358</v>
-      </c>
-      <c r="F27" t="s">
-        <v>358</v>
-      </c>
-      <c r="G27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" t="s">
-        <v>358</v>
-      </c>
-      <c r="I27" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2406,10 +2430,10 @@
         <v>149</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2424,7 +2448,7 @@
         <v>13</v>
       </c>
       <c r="H29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
@@ -2544,7 +2568,7 @@
         <v>11</v>
       </c>
       <c r="H33" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
@@ -2731,7 +2755,7 @@
         <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I39" t="s">
         <v>11</v>
@@ -3160,7 +3184,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D53" t="s">
         <v>13</v>
@@ -3181,7 +3205,7 @@
         <v>11</v>
       </c>
       <c r="L53" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3230,10 +3254,10 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D55" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -3653,7 +3677,7 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D71" t="s">
         <v>79</v>
@@ -3793,7 +3817,7 @@
         <v>13</v>
       </c>
       <c r="H75" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I75" t="s">
         <v>11</v>
@@ -3866,7 +3890,7 @@
         <v>11</v>
       </c>
       <c r="H77" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I77" t="s">
         <v>11</v>
@@ -3927,7 +3951,7 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D79" t="s">
         <v>79</v>
@@ -3936,7 +3960,7 @@
         <v>79</v>
       </c>
       <c r="F79" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G79" t="s">
         <v>13</v>
@@ -4076,22 +4100,22 @@
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D85" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E85" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F85" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G85" t="s">
         <v>13</v>
       </c>
       <c r="H85" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I85" t="s">
         <v>11</v>
@@ -4345,7 +4369,7 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D95" t="s">
         <v>79</v>
@@ -4480,7 +4504,7 @@
         <v>11</v>
       </c>
       <c r="L99" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -4529,7 +4553,7 @@
         <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D101" t="s">
         <v>13</v>
@@ -4776,12 +4800,32 @@
       <c r="A109" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="B109" s="3"/>
+      <c r="B109" s="3">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>373</v>
+      </c>
+      <c r="D109" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" t="s">
+        <v>13</v>
+      </c>
+      <c r="F109" t="s">
+        <v>13</v>
+      </c>
+      <c r="G109" t="s">
+        <v>13</v>
+      </c>
       <c r="H109" t="s">
         <v>352</v>
       </c>
       <c r="J109" t="s">
         <v>350</v>
+      </c>
+      <c r="K109" t="s">
+        <v>13</v>
       </c>
       <c r="L109" t="s">
         <v>351</v>
@@ -4829,7 +4873,27 @@
       <c r="A111" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B111" s="3"/>
+      <c r="B111" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C111" t="s">
+        <v>357</v>
+      </c>
+      <c r="D111" t="s">
+        <v>357</v>
+      </c>
+      <c r="E111" t="s">
+        <v>357</v>
+      </c>
+      <c r="F111" t="s">
+        <v>357</v>
+      </c>
+      <c r="G111" t="s">
+        <v>357</v>
+      </c>
+      <c r="H111" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
@@ -4873,7 +4937,33 @@
       <c r="A113" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="B113" s="3"/>
+      <c r="B113" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C113" t="s">
+        <v>278</v>
+      </c>
+      <c r="D113" t="s">
+        <v>11</v>
+      </c>
+      <c r="E113" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113" t="s">
+        <v>11</v>
+      </c>
+      <c r="H113" t="s">
+        <v>278</v>
+      </c>
+      <c r="I113" t="s">
+        <v>11</v>
+      </c>
+      <c r="L113" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
@@ -4961,7 +5051,36 @@
       <c r="A117" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="B117" s="3"/>
+      <c r="B117" s="3">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>357</v>
+      </c>
+      <c r="D117" t="s">
+        <v>13</v>
+      </c>
+      <c r="E117" t="s">
+        <v>357</v>
+      </c>
+      <c r="F117" t="s">
+        <v>11</v>
+      </c>
+      <c r="G117" t="s">
+        <v>13</v>
+      </c>
+      <c r="H117" t="s">
+        <v>374</v>
+      </c>
+      <c r="I117" t="s">
+        <v>11</v>
+      </c>
+      <c r="J117" t="s">
+        <v>25</v>
+      </c>
+      <c r="K117" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
@@ -5021,7 +5140,7 @@
         <v>13</v>
       </c>
       <c r="E120" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="F120" t="s">
         <v>11</v>
@@ -5049,7 +5168,27 @@
       <c r="A121" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B121" s="3"/>
+      <c r="B121" s="3">
+        <v>2</v>
+      </c>
+      <c r="C121" t="s">
+        <v>21</v>
+      </c>
+      <c r="D121" t="s">
+        <v>79</v>
+      </c>
+      <c r="E121" t="s">
+        <v>13</v>
+      </c>
+      <c r="F121" t="s">
+        <v>11</v>
+      </c>
+      <c r="G121" t="s">
+        <v>13</v>
+      </c>
+      <c r="I121" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
@@ -5109,7 +5248,7 @@
         <v>13</v>
       </c>
       <c r="E124" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="F124" t="s">
         <v>11</v>
@@ -5181,7 +5320,24 @@
       <c r="A127" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="B127" s="3"/>
+      <c r="B127" s="3">
+        <v>2</v>
+      </c>
+      <c r="C127" t="s">
+        <v>137</v>
+      </c>
+      <c r="D127" t="s">
+        <v>13</v>
+      </c>
+      <c r="E127" t="s">
+        <v>13</v>
+      </c>
+      <c r="F127" t="s">
+        <v>11</v>
+      </c>
+      <c r="G127" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
@@ -5225,7 +5381,24 @@
       <c r="A129" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="B129" s="3"/>
+      <c r="B129" s="3">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>375</v>
+      </c>
+      <c r="D129" t="s">
+        <v>13</v>
+      </c>
+      <c r="E129" t="s">
+        <v>13</v>
+      </c>
+      <c r="F129" t="s">
+        <v>13</v>
+      </c>
+      <c r="G129" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
@@ -5357,12 +5530,38 @@
       <c r="A135" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="B135" s="3"/>
+      <c r="B135" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C135" t="s">
+        <v>278</v>
+      </c>
+      <c r="D135" t="s">
+        <v>11</v>
+      </c>
+      <c r="E135" t="s">
+        <v>11</v>
+      </c>
+      <c r="F135" t="s">
+        <v>11</v>
+      </c>
+      <c r="G135" t="s">
+        <v>11</v>
+      </c>
+      <c r="H135" t="s">
+        <v>278</v>
+      </c>
+      <c r="I135" t="s">
+        <v>11</v>
+      </c>
       <c r="J135" t="s">
         <v>25</v>
       </c>
+      <c r="K135" t="s">
+        <v>11</v>
+      </c>
       <c r="L135" t="s">
-        <v>353</v>
+        <v>376</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -5420,13 +5619,13 @@
         <v>99</v>
       </c>
       <c r="D138" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E138" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F138" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G138" t="s">
         <v>13</v>
@@ -5451,7 +5650,39 @@
       <c r="A139" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="B139" s="3"/>
+      <c r="B139" s="3">
+        <v>2</v>
+      </c>
+      <c r="C139" t="s">
+        <v>377</v>
+      </c>
+      <c r="D139" t="s">
+        <v>13</v>
+      </c>
+      <c r="E139" t="s">
+        <v>13</v>
+      </c>
+      <c r="F139" t="s">
+        <v>13</v>
+      </c>
+      <c r="G139" t="s">
+        <v>13</v>
+      </c>
+      <c r="H139" t="s">
+        <v>378</v>
+      </c>
+      <c r="I139" t="s">
+        <v>11</v>
+      </c>
+      <c r="J139" t="s">
+        <v>35</v>
+      </c>
+      <c r="K139" t="s">
+        <v>11</v>
+      </c>
+      <c r="L139" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
@@ -5495,9 +5726,38 @@
       <c r="A141" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="B141" s="3"/>
+      <c r="B141" s="3">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>380</v>
+      </c>
+      <c r="D141" t="s">
+        <v>357</v>
+      </c>
+      <c r="E141" t="s">
+        <v>357</v>
+      </c>
+      <c r="F141" t="s">
+        <v>11</v>
+      </c>
+      <c r="G141" t="s">
+        <v>13</v>
+      </c>
+      <c r="H141" t="s">
+        <v>226</v>
+      </c>
+      <c r="I141" t="s">
+        <v>11</v>
+      </c>
+      <c r="J141" t="s">
+        <v>35</v>
+      </c>
+      <c r="K141" t="s">
+        <v>11</v>
+      </c>
       <c r="L141" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
@@ -5542,7 +5802,36 @@
       <c r="A143" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="B143" s="3"/>
+      <c r="B143" s="3">
+        <v>2</v>
+      </c>
+      <c r="C143" t="s">
+        <v>99</v>
+      </c>
+      <c r="D143" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" t="s">
+        <v>13</v>
+      </c>
+      <c r="F143" t="s">
+        <v>13</v>
+      </c>
+      <c r="G143" t="s">
+        <v>13</v>
+      </c>
+      <c r="H143" t="s">
+        <v>58</v>
+      </c>
+      <c r="I143" t="s">
+        <v>11</v>
+      </c>
+      <c r="J143" t="s">
+        <v>35</v>
+      </c>
+      <c r="K143" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
@@ -5586,7 +5875,36 @@
       <c r="A145" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="B145" s="3"/>
+      <c r="B145" s="3">
+        <v>2</v>
+      </c>
+      <c r="C145" t="s">
+        <v>99</v>
+      </c>
+      <c r="D145" t="s">
+        <v>13</v>
+      </c>
+      <c r="E145" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" t="s">
+        <v>13</v>
+      </c>
+      <c r="G145" t="s">
+        <v>13</v>
+      </c>
+      <c r="H145" t="s">
+        <v>58</v>
+      </c>
+      <c r="I145" t="s">
+        <v>11</v>
+      </c>
+      <c r="J145" t="s">
+        <v>35</v>
+      </c>
+      <c r="K145" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
@@ -5674,7 +5992,27 @@
       <c r="A149" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B149" s="3"/>
+      <c r="B149" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C149" t="s">
+        <v>357</v>
+      </c>
+      <c r="D149" t="s">
+        <v>357</v>
+      </c>
+      <c r="E149" t="s">
+        <v>357</v>
+      </c>
+      <c r="F149" t="s">
+        <v>11</v>
+      </c>
+      <c r="G149" t="s">
+        <v>13</v>
+      </c>
+      <c r="K149" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
@@ -5762,7 +6100,36 @@
       <c r="A153" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B153" s="3"/>
+      <c r="B153" s="3">
+        <v>2</v>
+      </c>
+      <c r="C153" t="s">
+        <v>99</v>
+      </c>
+      <c r="D153" t="s">
+        <v>13</v>
+      </c>
+      <c r="E153" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" t="s">
+        <v>11</v>
+      </c>
+      <c r="G153" t="s">
+        <v>13</v>
+      </c>
+      <c r="H153" t="s">
+        <v>22</v>
+      </c>
+      <c r="I153" t="s">
+        <v>11</v>
+      </c>
+      <c r="J153" t="s">
+        <v>35</v>
+      </c>
+      <c r="K153" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="3">

</xml_diff>